<commit_message>
Added changelog and ignore
</commit_message>
<xml_diff>
--- a/project_plan.xlsx
+++ b/project_plan.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,27 +425,27 @@
       <c r="A1" t="inlineStr"/>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Task Name</t>
+          <t xml:space="preserve"> Task Name </t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Duration</t>
+          <t xml:space="preserve"> Duration </t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Dependencies</t>
+          <t xml:space="preserve"> Dependencies </t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t xml:space="preserve"> Status </t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Resources</t>
+          <t xml:space="preserve"> Resources </t>
         </is>
       </c>
       <c r="G1" t="inlineStr"/>
@@ -483,27 +483,27 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Project Initiation</t>
+          <t xml:space="preserve"> Project Initiation &amp; Planning </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5 days</t>
+          <t xml:space="preserve"> 1 week </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t xml:space="preserve"> None </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Project Manager, Project Sponsor</t>
+          <t xml:space="preserve"> Project Manager </t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -512,27 +512,27 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Detailed Requirements Gathering</t>
+          <t xml:space="preserve"> Requirements Gathering &amp; Analysis </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t xml:space="preserve"> 2 weeks </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Project Initiation</t>
+          <t xml:space="preserve"> Project Initiation &amp; Planning </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Project Manager, Development Team</t>
+          <t xml:space="preserve"> Project Manager, Development Team </t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -541,27 +541,27 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Database Design</t>
+          <t xml:space="preserve"> System Architecture Design </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t xml:space="preserve"> 2 weeks </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Detailed Requirements Gathering</t>
+          <t xml:space="preserve"> Requirements Gathering &amp; Analysis </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Development Team</t>
+          <t xml:space="preserve"> Development Team </t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -570,27 +570,27 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>API Development</t>
+          <t xml:space="preserve"> UI/UX Design </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>45 days</t>
+          <t xml:space="preserve"> 3 weeks </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Database Design</t>
+          <t xml:space="preserve"> System Architecture Design </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Development Team</t>
+          <t xml:space="preserve"> UI/UX Designer </t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -599,27 +599,27 @@
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>iOS App Development</t>
+          <t xml:space="preserve"> Backend Development </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>90 days</t>
+          <t xml:space="preserve"> 12 weeks </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>API Development</t>
+          <t xml:space="preserve"> System Architecture Design </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Development Team</t>
+          <t xml:space="preserve"> Development Team </t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -628,27 +628,27 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Android App Development</t>
+          <t xml:space="preserve"> iOS App Development </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>90 days</t>
+          <t xml:space="preserve"> 10 weeks </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>API Development</t>
+          <t xml:space="preserve"> UI/UX Design, Backend Development </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Development Team</t>
+          <t xml:space="preserve"> iOS Development Team </t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -657,27 +657,27 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Payment Gateway Integration</t>
+          <t xml:space="preserve"> Android App Development </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>20 days</t>
+          <t xml:space="preserve"> 10 weeks </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>API Development</t>
+          <t xml:space="preserve"> UI/UX Design, Backend Development </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Development Team</t>
+          <t xml:space="preserve"> Android Development Team </t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -686,27 +686,27 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Testing and Quality Assurance</t>
+          <t xml:space="preserve"> Payment Gateway Integration </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>30 days</t>
+          <t xml:space="preserve"> 4 weeks </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>iOS App Development, Android App Development, Payment Gateway Integration</t>
+          <t xml:space="preserve"> Backend Development </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Development Team</t>
+          <t xml:space="preserve"> Development Team </t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -715,27 +715,27 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>User Guide and Help Documentation</t>
+          <t xml:space="preserve"> Quality Assurance &amp; Testing </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t xml:space="preserve"> 6 weeks </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Testing and Quality Assurance</t>
+          <t xml:space="preserve"> iOS App Development, Android App Development, Payment Gateway Integration </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t xml:space="preserve"> QA Team </t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -744,27 +744,27 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Deployment and Release Planning</t>
+          <t xml:space="preserve"> User Documentation &amp; Onboarding Guides </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t xml:space="preserve"> 2 weeks </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Testing and Quality Assurance</t>
+          <t xml:space="preserve"> Quality Assurance &amp; Testing </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Project Manager, Development Team</t>
+          <t xml:space="preserve"> Technical Writer </t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -773,27 +773,27 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>App Store Submission</t>
+          <t xml:space="preserve"> Deployment of Backend </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5 days</t>
+          <t xml:space="preserve"> 1 week </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Deployment and Release Planning</t>
+          <t xml:space="preserve"> Quality Assurance &amp; Testing </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t xml:space="preserve"> DevOps Team </t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -802,27 +802,27 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Marketing and Launch</t>
+          <t xml:space="preserve"> App Store Submission (iOS &amp; Android) </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>30 days</t>
+          <t xml:space="preserve"> 1 week </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>App Store Submission</t>
+          <t xml:space="preserve"> Quality Assurance &amp; Testing, Deployment of Backend </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Marketing Team, Project Manager</t>
+          <t xml:space="preserve"> Project Manager </t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -831,33 +831,91 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Post-Launch Monitoring &amp; Support</t>
+          <t xml:space="preserve"> Marketing &amp; Launch Preparation </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ongoing</t>
+          <t xml:space="preserve"> 4 weeks </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Marketing and Launch</t>
+          <t xml:space="preserve"> User Documentation &amp; Onboarding Guides, Deployment of Backend, App Store Submission (iOS &amp; Android) </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t xml:space="preserve"> Not Started </t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Development Team, Project Manager</t>
+          <t xml:space="preserve"> Marketing Team </t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Project Launch </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1 day </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Marketing &amp; Launch Preparation </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Not Started </t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Project Manager, Marketing Team </t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Post-Launch Monitoring &amp; Bug Fixes </t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ongoing </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Project Launch </t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Not Started </t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Development Team, QA Team </t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>